<commit_message>
Deep dive total run.
</commit_message>
<xml_diff>
--- a/Data/semi_clean/First100unlabeledIDV.xlsx
+++ b/Data/semi_clean/First100unlabeledIDV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Vendor\Data\semi_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16F64D-28A9-4D9D-A7B8-41AFE33AD6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2F7A95-10E3-41A0-91EB-CD64909004DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0EE5401E-0B10-4C85-801C-31A33C94C980}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="254">
   <si>
     <t>fiscal_year</t>
   </si>
@@ -749,13 +749,72 @@
   </si>
   <si>
     <t>IDV</t>
+  </si>
+  <si>
+    <t>IsDerived</t>
+  </si>
+  <si>
+    <t>HasParent</t>
+  </si>
+  <si>
+    <t>cauofferblank</t>
+  </si>
+  <si>
+    <t>pcauofferblank</t>
+  </si>
+  <si>
+    <t>ppcauofferblank</t>
+  </si>
+  <si>
+    <t>cauidvblank</t>
+  </si>
+  <si>
+    <t>pcauidvblank</t>
+  </si>
+  <si>
+    <t>ppcauidvblank</t>
+  </si>
+  <si>
+    <t>cauoidcblank</t>
+  </si>
+  <si>
+    <t>pcauidcblank</t>
+  </si>
+  <si>
+    <t>ppcauidcblank</t>
+  </si>
+  <si>
+    <t>cauomultiblank</t>
+  </si>
+  <si>
+    <t>pcaumultiblank</t>
+  </si>
+  <si>
+    <t>ppcaumultiblank</t>
+  </si>
+  <si>
+    <t>pcaucount</t>
+  </si>
+  <si>
+    <t>nonderivedpcaucount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,13 +840,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6164,15 +6226,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3A4FE1-8368-452E-806F-8979BE342419}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K3"/>
+      <selection activeCell="A5" sqref="A5:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -6207,7 +6269,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -6242,7 +6304,7 @@
         <v>15288915</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -6275,6 +6337,342 @@
       </c>
       <c r="K3">
         <v>198764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H5" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" t="s">
+        <v>245</v>
+      </c>
+      <c r="J5" t="s">
+        <v>246</v>
+      </c>
+      <c r="K5" t="s">
+        <v>247</v>
+      </c>
+      <c r="L5" t="s">
+        <v>248</v>
+      </c>
+      <c r="M5" t="s">
+        <v>249</v>
+      </c>
+      <c r="N5" t="s">
+        <v>250</v>
+      </c>
+      <c r="O5" t="s">
+        <v>251</v>
+      </c>
+      <c r="P5" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>252</v>
+      </c>
+      <c r="R5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4058</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4058</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4058</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2322539</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8264182</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4598638</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4478569</v>
+      </c>
+      <c r="G7" s="1">
+        <v>12966376</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7479678</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7346447</v>
+      </c>
+      <c r="J7" s="1">
+        <v>12966376</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9109364</v>
+      </c>
+      <c r="L7" s="1">
+        <v>9109364</v>
+      </c>
+      <c r="M7" s="1">
+        <v>226314</v>
+      </c>
+      <c r="N7" s="1">
+        <v>211370</v>
+      </c>
+      <c r="O7" s="1">
+        <v>211048</v>
+      </c>
+      <c r="P7" s="1">
+        <v>12966376</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>12966376</v>
+      </c>
+      <c r="R7" s="1">
+        <v>7734502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>55612</v>
+      </c>
+      <c r="E8" s="1">
+        <v>55612</v>
+      </c>
+      <c r="F8" s="1">
+        <v>55612</v>
+      </c>
+      <c r="G8" s="1">
+        <v>38334</v>
+      </c>
+      <c r="H8" s="1">
+        <v>38334</v>
+      </c>
+      <c r="I8" s="1">
+        <v>38334</v>
+      </c>
+      <c r="J8" s="1">
+        <v>74164</v>
+      </c>
+      <c r="K8" s="1">
+        <v>74164</v>
+      </c>
+      <c r="L8" s="1">
+        <v>74164</v>
+      </c>
+      <c r="M8" s="1">
+        <v>38422</v>
+      </c>
+      <c r="N8" s="1">
+        <v>38422</v>
+      </c>
+      <c r="O8" s="1">
+        <v>38422</v>
+      </c>
+      <c r="P8" s="1">
+        <v>130813</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2326</v>
+      </c>
+      <c r="E9" s="1">
+        <v>559</v>
+      </c>
+      <c r="F9" s="1">
+        <v>559</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2307</v>
+      </c>
+      <c r="H9" s="1">
+        <v>528</v>
+      </c>
+      <c r="I9" s="1">
+        <v>528</v>
+      </c>
+      <c r="J9" s="1">
+        <v>7034</v>
+      </c>
+      <c r="K9" s="1">
+        <v>7034</v>
+      </c>
+      <c r="L9" s="1">
+        <v>7034</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2310</v>
+      </c>
+      <c r="N9" s="1">
+        <v>528</v>
+      </c>
+      <c r="O9" s="1">
+        <v>528</v>
+      </c>
+      <c r="P9" s="1">
+        <v>7034</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>6991</v>
+      </c>
+      <c r="R9" s="1">
+        <v>6521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="E10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="F10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="G10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="H10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="I10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="J10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="K10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="L10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="M10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="N10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="O10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="P10" s="1">
+        <v>60917</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>